<commit_message>
css for produktside og index + kommentarer på klare unødvendige deler av WCAG
</commit_message>
<xml_diff>
--- a/Eksamen/Mal – WCAG-sjekkliste for utfylling av tilgjengelighetserklæring for nettløsning 24.01.2024.xlsx
+++ b/Eksamen/Mal – WCAG-sjekkliste for utfylling av tilgjengelighetserklæring for nettløsning 24.01.2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivro1\Documents\Eksamen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50921340-666F-44CA-8D12-462C7F1B9B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359FAF03-0F97-4669-8F09-D0FEDDEB6BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="100">
   <si>
     <t>Oversikt over status for universell utforming i én enkelt nettløsning. Her ser du WCAG-kravene som nettsteder skal oppfylle, sortert på de fire prinsippene i WCAG-standarden. For hver av retningslinjene finnes beskrivelser, lenker til mer informasjon, m.m., samt en nedtrekksmeny der du kan notere status pr i dag.
 Du kan laste ned arket og bruke det som arbeidsliste, men følg alltid med på uutilsynet.no for oppdatert kravliste.</t>
@@ -330,6 +330,12 @@
   </si>
   <si>
     <t>Innholdet er kun visuelt med bruk av tekst og linker til sider.</t>
+  </si>
+  <si>
+    <t>Teksten på sidene er skrevet inn med forskjellig semantiske tagger og ikke bilder</t>
+  </si>
+  <si>
+    <t>Nettsiden har en maks på 1200px basert på oppgavekrav</t>
   </si>
 </sst>
 </file>
@@ -1730,10 +1736,10 @@
   <dimension ref="A1:O997"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2195,9 +2201,11 @@
         <v>28</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="7" t="s">
+        <v>98</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -2216,9 +2224,11 @@
         <v>29</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="7" t="s">
+        <v>99</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -2279,7 +2289,7 @@
         <v>32</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="1"/>

</xml_diff>